<commit_message>
Logo changes across forms
</commit_message>
<xml_diff>
--- a/ILRG_ORAM_A_pontos/ILRG_ORAM_A_pontos-media/ILRG_ORAM_A_pontos.xlsx
+++ b/ILRG_ORAM_A_pontos/ILRG_ORAM_A_pontos-media/ILRG_ORAM_A_pontos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\Grants\Dams project\ODK Forms\ILRG_ORAM_odk_forms\ILRG_ORAM_A_pontos\ILRG_ORAM_A_pontos-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B789D150-EF23-45BC-9377-8BFDF9BFB30B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9858F856-E4F9-4ABA-B09A-950BB59EB6CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="327">
   <si>
     <t>type</t>
   </si>
@@ -176,9 +176,6 @@
     <t xml:space="preserve">image </t>
   </si>
   <si>
-    <t>poi_picture</t>
-  </si>
-  <si>
     <t>no-calendar</t>
   </si>
   <si>
@@ -890,13 +887,7 @@
     <t>logo</t>
   </si>
   <si>
-    <t>form_logo.jpg</t>
-  </si>
-  <si>
     <t>cavateco</t>
-  </si>
-  <si>
-    <t>&lt;br/&gt; &lt;h1&gt;A Cadeia de Valor de Terra Comunitária&lt;/h1&gt;&lt;br/&gt; &lt;h2&gt;Uma iniciativa da Terra Firma&lt;/h2&gt;&lt;span style="color:#57b055"&gt;${my_form_name}&lt;/span&gt; &lt;br/&gt;</t>
   </si>
   <si>
     <t>Ag3</t>
@@ -980,9 +971,6 @@
 Por favor deslizar para a frente para continuar.</t>
   </si>
   <si>
-    <t>Inicio</t>
-  </si>
-  <si>
     <t>ILRG ORAM A - Gravar Pontos de Interesse</t>
   </si>
   <si>
@@ -1019,16 +1007,39 @@
     <t>-</t>
   </si>
   <si>
-    <t>&lt;h2&gt;Introduza o seu nome&lt;/h2&gt;&lt;br&gt;&lt;br&gt;Nome do(a) técnico(a):</t>
+    <t>oram_USAID.jpg</t>
+  </si>
+  <si>
+    <t>&lt;br/&gt; &lt;h1&gt;Projecto de Governação Integrada de Terra e Recursos&lt;/h1&gt;&lt;br/&gt; &lt;h2&gt;Uma iniciativa da USAID implementada pela ORAM e Terra Firma&lt;/h2&gt;&lt;span style="color:#57b055"&gt;${my_form_name}&lt;/span&gt; &lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Introduza o seu nome&lt;br&gt;Nome do(a) técnico(a):</t>
+  </si>
+  <si>
+    <t>image_poi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1338,393 +1349,394 @@
   </borders>
   <cellStyleXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -2306,17 +2318,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.25" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.25" style="51" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91.375" style="5" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="11.5" style="5" bestFit="1" customWidth="1"/>
@@ -2388,129 +2400,127 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
-        <v>325</v>
-      </c>
-      <c r="B4" s="78" t="s">
-        <v>325</v>
-      </c>
-      <c r="C4" s="77" t="s">
-        <v>326</v>
+    <row r="4" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
+        <v>321</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>321</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>164</v>
-      </c>
-      <c r="M5" s="69" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="67" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="L6" s="65" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="66" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="L6" s="64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="N7" s="77" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="65" t="s">
         <v>285</v>
       </c>
-      <c r="N7" s="65" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="66" t="s">
-        <v>287</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="78" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="66"/>
+        <v>116</v>
+      </c>
+      <c r="B9" s="65"/>
     </row>
     <row r="10" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="72" t="s">
-        <v>313</v>
+      <c r="C10" s="70" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>327</v>
+        <v>49</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>325</v>
       </c>
       <c r="J11" s="17" t="s">
         <v>22</v>
       </c>
       <c r="L11" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="G12" s="56" t="s">
-        <v>174</v>
+        <v>276</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>173</v>
       </c>
       <c r="L12" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="76" t="s">
-        <v>320</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="H13" s="53" t="s">
-        <v>165</v>
-      </c>
-      <c r="J13" s="56" t="s">
+      <c r="B13" s="74" t="s">
+        <v>316</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="H13" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="J13" s="55" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2518,23 +2528,23 @@
       <c r="A14" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="76" t="s">
-        <v>321</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>173</v>
-      </c>
-      <c r="G14" s="56"/>
-      <c r="H14" s="53" t="s">
-        <v>165</v>
-      </c>
-      <c r="J14" s="56" t="s">
+      <c r="B14" s="74" t="s">
+        <v>317</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="G14" s="55"/>
+      <c r="H14" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="J14" s="55" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="46"/>
       <c r="C15" s="23"/>
@@ -2544,31 +2554,31 @@
       <c r="A16" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="56" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J16" s="17" t="s">
         <v>22</v>
       </c>
       <c r="L16" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="76" t="s">
-        <v>322</v>
+      <c r="B17" s="74" t="s">
+        <v>318</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="69" t="s">
-        <v>292</v>
+      <c r="F17" s="67" t="s">
+        <v>289</v>
       </c>
       <c r="G17" s="13"/>
       <c r="J17" s="15" t="s">
@@ -2577,37 +2587,37 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>62</v>
       </c>
       <c r="G18" s="13"/>
       <c r="J18" s="15" t="s">
         <v>22</v>
       </c>
       <c r="L18" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="57" t="s">
-        <v>175</v>
+      <c r="B19" s="56" t="s">
+        <v>174</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="56" t="s">
-        <v>200</v>
-      </c>
-      <c r="H19" s="53" t="s">
-        <v>166</v>
+        <v>62</v>
+      </c>
+      <c r="G19" s="55" t="s">
+        <v>199</v>
+      </c>
+      <c r="H19" s="52" t="s">
+        <v>165</v>
       </c>
       <c r="J19" s="22" t="s">
         <v>22</v>
@@ -2617,7 +2627,7 @@
       <c r="A20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="56" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -2628,21 +2638,21 @@
         <v>22</v>
       </c>
       <c r="L20" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="56" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="55" t="s">
         <v>198</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" s="56" t="s">
-        <v>199</v>
       </c>
       <c r="J21" s="15"/>
     </row>
@@ -2650,14 +2660,14 @@
       <c r="A22" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="57" t="s">
-        <v>215</v>
+      <c r="B22" s="56" t="s">
+        <v>214</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="56" t="s">
-        <v>201</v>
+        <v>70</v>
+      </c>
+      <c r="G22" s="55" t="s">
+        <v>200</v>
       </c>
       <c r="J22" s="15"/>
     </row>
@@ -2665,14 +2675,14 @@
       <c r="A23" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="57" t="s">
-        <v>216</v>
+      <c r="B23" s="56" t="s">
+        <v>215</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="56" t="s">
-        <v>202</v>
+        <v>71</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>201</v>
       </c>
       <c r="J23" s="15"/>
     </row>
@@ -2680,14 +2690,14 @@
       <c r="A24" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="57" t="s">
-        <v>217</v>
+      <c r="B24" s="56" t="s">
+        <v>216</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="56" t="s">
-        <v>205</v>
+        <v>72</v>
+      </c>
+      <c r="G24" s="55" t="s">
+        <v>204</v>
       </c>
       <c r="J24" s="15"/>
     </row>
@@ -2695,14 +2705,14 @@
       <c r="A25" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="48" t="s">
-        <v>55</v>
+      <c r="B25" s="47" t="s">
+        <v>54</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="56" t="s">
-        <v>206</v>
+        <v>58</v>
+      </c>
+      <c r="G25" s="55" t="s">
+        <v>205</v>
       </c>
       <c r="J25" s="22"/>
     </row>
@@ -2710,14 +2720,14 @@
       <c r="A26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="57" t="s">
-        <v>218</v>
+      <c r="B26" s="56" t="s">
+        <v>217</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="G26" s="56" t="s">
-        <v>207</v>
+        <v>82</v>
+      </c>
+      <c r="G26" s="55" t="s">
+        <v>206</v>
       </c>
       <c r="J26" s="22"/>
     </row>
@@ -2725,14 +2735,14 @@
       <c r="A27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="57" t="s">
-        <v>219</v>
+      <c r="B27" s="56" t="s">
+        <v>218</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" s="56" t="s">
-        <v>208</v>
+        <v>83</v>
+      </c>
+      <c r="G27" s="55" t="s">
+        <v>207</v>
       </c>
       <c r="J27" s="22"/>
     </row>
@@ -2740,14 +2750,14 @@
       <c r="A28" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="C28" s="56" t="s">
+      <c r="B28" s="56" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="G28" s="55" t="s">
         <v>212</v>
-      </c>
-      <c r="G28" s="56" t="s">
-        <v>213</v>
       </c>
       <c r="J28" s="22"/>
     </row>
@@ -2755,14 +2765,14 @@
       <c r="A29" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="57" t="s">
-        <v>220</v>
+      <c r="B29" s="56" t="s">
+        <v>219</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="G29" s="56" t="s">
-        <v>209</v>
+        <v>84</v>
+      </c>
+      <c r="G29" s="55" t="s">
+        <v>208</v>
       </c>
       <c r="J29" s="22"/>
     </row>
@@ -2770,138 +2780,138 @@
       <c r="A30" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="57" t="s">
-        <v>221</v>
+      <c r="B30" s="56" t="s">
+        <v>220</v>
       </c>
       <c r="C30" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="30" t="s">
         <v>87</v>
-      </c>
-      <c r="G30" s="30" t="s">
-        <v>88</v>
       </c>
       <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="57" t="s">
-        <v>224</v>
+        <v>74</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>223</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="G31" s="56" t="s">
-        <v>211</v>
+        <v>73</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>210</v>
       </c>
       <c r="J31" s="22"/>
       <c r="L31" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="56" t="s">
+        <v>221</v>
+      </c>
+      <c r="C32" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="57" t="s">
-        <v>222</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="G32" s="56" t="s">
-        <v>232</v>
+      <c r="G32" s="55" t="s">
+        <v>231</v>
       </c>
       <c r="J32" s="39" t="s">
         <v>22</v>
       </c>
       <c r="L32" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="57" t="s">
-        <v>223</v>
+      <c r="B33" s="56" t="s">
+        <v>222</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="56" t="s">
-        <v>276</v>
+        <v>102</v>
+      </c>
+      <c r="G33" s="55" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="57" t="s">
-        <v>233</v>
-      </c>
-      <c r="C34" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="G34" s="56" t="s">
-        <v>232</v>
+      <c r="G34" s="55" t="s">
+        <v>231</v>
       </c>
       <c r="J34" s="39" t="s">
         <v>22</v>
       </c>
       <c r="L34" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="56" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="57" t="s">
-        <v>234</v>
-      </c>
-      <c r="C35" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35" s="56" t="s">
-        <v>232</v>
+      <c r="G35" s="55" t="s">
+        <v>231</v>
       </c>
       <c r="J35" s="39" t="s">
         <v>22</v>
       </c>
       <c r="L35" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="57" t="s">
-        <v>235</v>
+      <c r="B36" s="56" t="s">
+        <v>234</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="G36" s="67" t="s">
-        <v>290</v>
-      </c>
-      <c r="H36" s="53" t="s">
-        <v>166</v>
+        <v>107</v>
+      </c>
+      <c r="G36" s="66" t="s">
+        <v>287</v>
+      </c>
+      <c r="H36" s="52" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="57" t="s">
-        <v>157</v>
+        <v>60</v>
+      </c>
+      <c r="B37" s="56" t="s">
+        <v>156</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="56" t="s">
-        <v>232</v>
+        <v>108</v>
+      </c>
+      <c r="G37" s="55" t="s">
+        <v>231</v>
       </c>
       <c r="J37" s="39" t="s">
         <v>22</v>
@@ -2909,70 +2919,70 @@
     </row>
     <row r="38" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="34" t="s">
-        <v>289</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="G38" s="55" t="s">
+        <v>241</v>
+      </c>
+      <c r="L38" s="39" t="s">
         <v>111</v>
-      </c>
-      <c r="G38" s="56" t="s">
-        <v>242</v>
-      </c>
-      <c r="L38" s="39" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="C39" s="39" t="s">
         <v>113</v>
-      </c>
-      <c r="B39" s="57" t="s">
-        <v>238</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>114</v>
       </c>
       <c r="J39" s="39" t="s">
         <v>22</v>
       </c>
       <c r="L39" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="56" t="s">
+        <v>238</v>
+      </c>
+      <c r="C40" s="39" t="s">
         <v>115</v>
-      </c>
-      <c r="B40" s="57" t="s">
-        <v>239</v>
-      </c>
-      <c r="C40" s="39" t="s">
-        <v>116</v>
       </c>
       <c r="J40" s="39" t="s">
         <v>22</v>
       </c>
       <c r="L40" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="49"/>
+        <v>116</v>
+      </c>
+      <c r="B41" s="48"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="47" t="s">
-        <v>48</v>
+      <c r="B42" s="79" t="s">
+        <v>326</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G42" s="13"/>
       <c r="J42" s="15"/>
@@ -3013,7 +3023,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="50"/>
+      <c r="B48" s="49"/>
       <c r="C48" s="14"/>
       <c r="F48" s="14"/>
       <c r="G48" s="13"/>
@@ -3021,76 +3031,76 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
-      <c r="B49" s="50"/>
+      <c r="B49" s="49"/>
       <c r="C49" s="14"/>
       <c r="G49" s="13"/>
       <c r="J49" s="14"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="B50" s="50"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="13"/>
       <c r="G50" s="13"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="50"/>
+      <c r="B51" s="49"/>
       <c r="C51" s="14"/>
       <c r="G51" s="13"/>
       <c r="J51" s="14"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
-      <c r="B52" s="50"/>
+      <c r="B52" s="49"/>
       <c r="C52" s="14"/>
       <c r="G52" s="14"/>
       <c r="J52" s="14"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
-      <c r="B53" s="50"/>
+      <c r="B53" s="49"/>
       <c r="C53" s="14"/>
       <c r="G53" s="13"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="50"/>
+      <c r="B54" s="49"/>
       <c r="C54" s="14"/>
       <c r="G54" s="13"/>
       <c r="J54" s="14"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
-      <c r="B55" s="50"/>
+      <c r="B55" s="49"/>
       <c r="C55" s="14"/>
       <c r="G55" s="14"/>
       <c r="J55" s="14"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="50"/>
+      <c r="B56" s="49"/>
       <c r="C56" s="14"/>
       <c r="J56" s="14"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
-      <c r="B57" s="50"/>
+      <c r="B57" s="49"/>
       <c r="C57" s="14"/>
       <c r="G57" s="14"/>
       <c r="J57" s="14"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="50"/>
+      <c r="B58" s="49"/>
       <c r="C58" s="14"/>
       <c r="J58" s="14"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
-      <c r="B59" s="50"/>
+      <c r="B59" s="49"/>
       <c r="C59" s="14"/>
       <c r="G59" s="14"/>
       <c r="J59" s="14"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
-      <c r="B60" s="50"/>
+      <c r="B60" s="49"/>
       <c r="C60" s="14"/>
       <c r="G60" s="13"/>
     </row>
@@ -3100,35 +3110,35 @@
       <c r="C61" s="13"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="51"/>
+      <c r="B62" s="50"/>
       <c r="C62" s="14"/>
       <c r="J62" s="13"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="51"/>
+      <c r="B63" s="50"/>
       <c r="C63" s="14"/>
       <c r="J63" s="13"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
-      <c r="B64" s="50"/>
+      <c r="B64" s="49"/>
       <c r="C64" s="13"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="50"/>
+      <c r="B65" s="49"/>
       <c r="C65" s="13"/>
       <c r="J65" s="14"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="50"/>
+      <c r="B66" s="49"/>
       <c r="C66" s="13"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="50"/>
+      <c r="B67" s="49"/>
       <c r="C67" s="13"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="50"/>
+      <c r="B68" s="49"/>
       <c r="C68" s="13"/>
       <c r="F68" s="14"/>
       <c r="J68" s="14"/>
@@ -3144,7 +3154,7 @@
   <dimension ref="A1:H107"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
@@ -3187,11 +3197,11 @@
       <c r="A3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>303</v>
-      </c>
-      <c r="C3" s="74" t="s">
-        <v>319</v>
+      <c r="B3" s="57" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>315</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="3"/>
@@ -3201,11 +3211,11 @@
       <c r="A4" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="58" t="s">
-        <v>304</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>298</v>
+      <c r="B4" s="57" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="69" t="s">
+        <v>295</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
@@ -3215,11 +3225,11 @@
       <c r="A5" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="58" t="s">
-        <v>305</v>
-      </c>
-      <c r="C5" s="70" t="s">
-        <v>295</v>
+      <c r="B5" s="57" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>292</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -3229,11 +3239,11 @@
       <c r="A6" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="58" t="s">
-        <v>306</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>301</v>
+      <c r="B6" s="57" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" s="69" t="s">
+        <v>298</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
@@ -3243,11 +3253,11 @@
       <c r="A7" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="75" t="s">
-        <v>318</v>
-      </c>
-      <c r="C7" s="74" t="s">
-        <v>317</v>
+      <c r="B7" s="73" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>313</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
@@ -3257,11 +3267,11 @@
       <c r="A8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="58" t="s">
-        <v>307</v>
-      </c>
-      <c r="C8" s="71" t="s">
-        <v>300</v>
+      <c r="B8" s="57" t="s">
+        <v>304</v>
+      </c>
+      <c r="C8" s="69" t="s">
+        <v>297</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
@@ -3271,11 +3281,11 @@
       <c r="A9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="75" t="s">
-        <v>323</v>
-      </c>
-      <c r="C9" s="70" t="s">
-        <v>294</v>
+      <c r="B9" s="73" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>291</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
@@ -3285,11 +3295,11 @@
       <c r="A10" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="58" t="s">
-        <v>308</v>
-      </c>
-      <c r="C10" s="70" t="s">
-        <v>293</v>
+      <c r="B10" s="57" t="s">
+        <v>305</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>290</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
@@ -3299,11 +3309,11 @@
       <c r="A11" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="58" t="s">
-        <v>309</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>299</v>
+      <c r="B11" s="57" t="s">
+        <v>306</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>296</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
@@ -3313,11 +3323,11 @@
       <c r="A12" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="58" t="s">
-        <v>310</v>
-      </c>
-      <c r="C12" s="70" t="s">
-        <v>296</v>
+      <c r="B12" s="57" t="s">
+        <v>307</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>293</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
@@ -3327,33 +3337,33 @@
       <c r="A13" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="75" t="s">
-        <v>324</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>297</v>
+      <c r="B13" s="73" t="s">
+        <v>320</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="58" t="s">
-        <v>311</v>
-      </c>
-      <c r="C14" s="71" t="s">
-        <v>302</v>
+      <c r="B14" s="57" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" s="69" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="58" t="s">
-        <v>170</v>
+      <c r="B15" s="57" t="s">
+        <v>169</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3363,7 +3373,7 @@
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="57" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -3375,8 +3385,8 @@
       <c r="A18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="58" t="s">
-        <v>171</v>
+      <c r="B18" s="57" t="s">
+        <v>170</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>25</v>
@@ -3385,7 +3395,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="C19" s="59"/>
+      <c r="C19" s="58"/>
       <c r="E19" s="6"/>
       <c r="H19" s="26"/>
     </row>
@@ -3393,8 +3403,8 @@
       <c r="A20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="58" t="s">
-        <v>176</v>
+      <c r="B20" s="57" t="s">
+        <v>175</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>44</v>
@@ -3405,8 +3415,8 @@
       <c r="A21" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="58" t="s">
-        <v>177</v>
+      <c r="B21" s="57" t="s">
+        <v>176</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>45</v>
@@ -3414,14 +3424,14 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="C22" s="54" t="s">
+      <c r="B22" s="54" t="s">
         <v>167</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>166</v>
       </c>
       <c r="E22" s="6"/>
     </row>
@@ -3429,8 +3439,8 @@
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="58" t="s">
-        <v>179</v>
+      <c r="B23" s="57" t="s">
+        <v>178</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>43</v>
@@ -3441,11 +3451,11 @@
       <c r="A24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="C24" s="60" t="s">
-        <v>57</v>
+      <c r="B24" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="59" t="s">
+        <v>56</v>
       </c>
       <c r="E24" s="6"/>
     </row>
@@ -3453,11 +3463,11 @@
       <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="C25" s="73" t="s">
-        <v>312</v>
+      <c r="B25" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="71" t="s">
+        <v>309</v>
       </c>
       <c r="E25" s="6"/>
     </row>
@@ -3465,10 +3475,10 @@
       <c r="A26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="58" t="s">
-        <v>181</v>
-      </c>
-      <c r="C26" s="61" t="s">
+      <c r="B26" s="57" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" s="60" t="s">
         <v>41</v>
       </c>
       <c r="E26" s="6"/>
@@ -3477,8 +3487,8 @@
       <c r="A27" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="58" t="s">
-        <v>182</v>
+      <c r="B27" s="57" t="s">
+        <v>181</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>37</v>
@@ -3489,11 +3499,11 @@
       <c r="A28" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="58" t="s">
-        <v>76</v>
+      <c r="B28" s="57" t="s">
+        <v>75</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" s="6"/>
     </row>
@@ -3502,10 +3512,10 @@
         <v>33</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="62" t="s">
-        <v>210</v>
+        <v>85</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>209</v>
       </c>
       <c r="E29" s="6"/>
     </row>
@@ -3513,11 +3523,11 @@
       <c r="A30" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="58" t="s">
-        <v>183</v>
+      <c r="B30" s="57" t="s">
+        <v>182</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="6"/>
     </row>
@@ -3525,8 +3535,8 @@
       <c r="A31" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="58" t="s">
-        <v>184</v>
+      <c r="B31" s="57" t="s">
+        <v>183</v>
       </c>
       <c r="C31" s="16" t="s">
         <v>42</v>
@@ -3536,8 +3546,8 @@
       <c r="A32" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="58" t="s">
-        <v>185</v>
+      <c r="B32" s="57" t="s">
+        <v>184</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>36</v>
@@ -3547,8 +3557,8 @@
       <c r="A33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="58" t="s">
-        <v>186</v>
+      <c r="B33" s="57" t="s">
+        <v>185</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>34</v>
@@ -3558,30 +3568,30 @@
       <c r="A34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="C34" s="61" t="s">
         <v>203</v>
-      </c>
-      <c r="C34" s="62" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="58" t="s">
-        <v>197</v>
+      <c r="B35" s="57" t="s">
+        <v>196</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="58" t="s">
-        <v>187</v>
+      <c r="B36" s="57" t="s">
+        <v>186</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>38</v>
@@ -3591,8 +3601,8 @@
       <c r="A37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="58" t="s">
-        <v>188</v>
+      <c r="B37" s="57" t="s">
+        <v>187</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>39</v>
@@ -3602,19 +3612,19 @@
       <c r="A38" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="C38" s="63" t="s">
-        <v>82</v>
+      <c r="B38" s="57" t="s">
+        <v>188</v>
+      </c>
+      <c r="C38" s="62" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="58" t="s">
-        <v>190</v>
+      <c r="B39" s="57" t="s">
+        <v>189</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>46</v>
@@ -3624,8 +3634,8 @@
       <c r="A40" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="58" t="s">
-        <v>191</v>
+      <c r="B40" s="57" t="s">
+        <v>190</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>40</v>
@@ -3635,8 +3645,8 @@
       <c r="A41" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="58" t="s">
-        <v>192</v>
+      <c r="B41" s="57" t="s">
+        <v>191</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>35</v>
@@ -3646,55 +3656,55 @@
       <c r="A42" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="C42" s="60" t="s">
-        <v>58</v>
+      <c r="B42" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="58" t="s">
-        <v>194</v>
+      <c r="B43" s="57" t="s">
+        <v>193</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="C44" s="64" t="s">
-        <v>66</v>
+      <c r="B44" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" s="63" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="58" t="s">
-        <v>196</v>
+      <c r="B45" s="57" t="s">
+        <v>195</v>
       </c>
       <c r="C45" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="58" t="s">
-        <v>170</v>
+      <c r="B46" s="57" t="s">
+        <v>169</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3703,332 +3713,332 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48" s="62" t="s">
-        <v>279</v>
+      <c r="C48" s="61" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="62" t="s">
-        <v>280</v>
+        <v>77</v>
+      </c>
+      <c r="C49" s="61" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" s="62" t="s">
-        <v>281</v>
+        <v>78</v>
+      </c>
+      <c r="C50" s="61" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C51" s="62" t="s">
-        <v>282</v>
+        <v>79</v>
+      </c>
+      <c r="C51" s="61" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="62" t="s">
-        <v>283</v>
+        <v>80</v>
+      </c>
+      <c r="C52" s="61" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" s="57" t="s">
+        <v>224</v>
+      </c>
+      <c r="C54" s="33" t="s">
         <v>91</v>
-      </c>
-      <c r="B54" s="58" t="s">
-        <v>225</v>
-      </c>
-      <c r="C54" s="33" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B55" s="58" t="s">
-        <v>284</v>
+        <v>90</v>
+      </c>
+      <c r="B55" s="57" t="s">
+        <v>283</v>
       </c>
       <c r="C55" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B56" s="58" t="s">
-        <v>226</v>
+        <v>90</v>
+      </c>
+      <c r="B56" s="57" t="s">
+        <v>225</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" s="58" t="s">
-        <v>227</v>
+        <v>90</v>
+      </c>
+      <c r="B57" s="57" t="s">
+        <v>226</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="58" t="s">
-        <v>228</v>
+        <v>90</v>
+      </c>
+      <c r="B58" s="57" t="s">
+        <v>227</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B59" s="58" t="s">
-        <v>229</v>
+        <v>90</v>
+      </c>
+      <c r="B59" s="57" t="s">
+        <v>228</v>
       </c>
       <c r="C59" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" s="58" t="s">
-        <v>231</v>
+        <v>90</v>
+      </c>
+      <c r="B60" s="57" t="s">
+        <v>230</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B61" s="58" t="s">
-        <v>230</v>
+        <v>90</v>
+      </c>
+      <c r="B61" s="57" t="s">
+        <v>229</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="B62" s="58" t="s">
-        <v>170</v>
+        <v>90</v>
+      </c>
+      <c r="B62" s="57" t="s">
+        <v>169</v>
       </c>
       <c r="C62" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="33" t="s">
         <v>118</v>
-      </c>
-      <c r="B64" s="38" t="s">
-        <v>187</v>
-      </c>
-      <c r="C64" s="33" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C65" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B66" s="38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B68" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B69" s="38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B70" s="38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C70" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B71" s="38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B72" s="38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C72" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B73" s="38" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C73" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B74" s="38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C74" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B75" s="38" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C75" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C76" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B78" s="38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B79" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -4038,233 +4048,233 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B81" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="C81" s="33" t="s">
         <v>135</v>
-      </c>
-      <c r="B81" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="C81" s="33" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B82" s="38" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C82" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B83" s="38" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C84" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B85" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C85" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C86" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B87" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C87" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B88" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C88" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C89" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B90" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C90" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B91" s="58" t="s">
-        <v>274</v>
+        <v>134</v>
+      </c>
+      <c r="B91" s="57" t="s">
+        <v>273</v>
       </c>
       <c r="C91" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B92" s="38" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C92" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C93" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B94" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C94" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B95" s="38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C95" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B96" s="38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C96" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B97" s="58" t="s">
-        <v>275</v>
+        <v>134</v>
+      </c>
+      <c r="B97" s="57" t="s">
+        <v>274</v>
       </c>
       <c r="C97" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B98" s="38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C98" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B99" s="38" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C99" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B100" s="38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C100" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B101" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C101" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -4274,24 +4284,24 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B103" s="57" t="s">
+        <v>240</v>
+      </c>
+      <c r="C103" s="33" t="s">
         <v>157</v>
-      </c>
-      <c r="B103" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="C103" s="33" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B104" s="58" t="s">
-        <v>240</v>
+        <v>156</v>
+      </c>
+      <c r="B104" s="57" t="s">
+        <v>239</v>
       </c>
       <c r="C104" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -4301,24 +4311,24 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B106" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="C106" s="33" t="s">
         <v>160</v>
-      </c>
-      <c r="B106" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="C106" s="33" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B107" s="38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C107" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -4334,8 +4344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4355,7 +4365,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>23</v>
@@ -4363,16 +4373,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C2" s="31">
-        <v>201902271</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>278</v>
+        <v>201902282</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>